<commit_message>
fix lại báo cáo export
</commit_message>
<xml_diff>
--- a/DMS/Templates/Report_Direct_Sales_Order_By_Store_And_Item.xlsx
+++ b/DMS/Templates/Report_Direct_Sales_Order_By_Store_And_Item.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2FDFB0-0A1B-4882-8B6E-03B438662686}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D459C7-4CD6-4CD1-BF5C-D486C6044727}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -132,9 +132,6 @@
     <t>Địa chỉ đại lý</t>
   </si>
   <si>
-    <t>{{ReportSalesOrderByStoreAndItems.Stores.Items.SalesOrderCounter}}</t>
-  </si>
-  <si>
     <t>Trạng thái đại lý</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>BÁO CÁO BÁN HÀNG TRỰC TIẾP THEO ĐẠI LÝ VÀ SẢN PHẨM</t>
+  </si>
+  <si>
+    <t>{{ReportSalesOrderByStoreAndItems.Stores.Items.DirectSalesOrderCounter}}</t>
   </si>
 </sst>
 </file>
@@ -286,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -315,18 +315,18 @@
     <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -344,6 +344,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -627,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:U4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,7 +695,7 @@
     </row>
     <row r="4" spans="1:24" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -738,30 +741,30 @@
       <c r="R5" s="4"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="10" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="10" t="s">
+      <c r="F7" s="13"/>
+      <c r="G7" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="10" t="s">
+      <c r="H7" s="13"/>
+      <c r="I7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="13"/>
+      <c r="K7" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="L7" s="11"/>
+      <c r="L7" s="13"/>
       <c r="M7" s="1" t="s">
         <v>1</v>
       </c>
@@ -790,7 +793,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>16</v>
       </c>
@@ -813,36 +816,36 @@
       <c r="R8" s="18"/>
       <c r="S8" s="18"/>
       <c r="T8" s="18"/>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18"/>
-      <c r="W8" s="18"/>
-      <c r="X8" s="19"/>
+      <c r="U8" s="19"/>
+      <c r="V8" s="20"/>
+      <c r="W8" s="20"/>
+      <c r="X8" s="20"/>
     </row>
     <row r="9" spans="1:24" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="12" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="12" t="s">
+      <c r="D9" s="11"/>
+      <c r="E9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="11"/>
+      <c r="I9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="12" t="s">
+      <c r="J9" s="11"/>
+      <c r="K9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="L9" s="13"/>
+      <c r="L9" s="11"/>
       <c r="M9" s="7" t="s">
         <v>17</v>
       </c>
@@ -868,7 +871,7 @@
         <v>24</v>
       </c>
       <c r="U9" s="8" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="42.75" x14ac:dyDescent="0.25">
@@ -906,22 +909,22 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A4:U4"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="A8:U8"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="A10:O10"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="A4:U4"/>
-    <mergeCell ref="A8:X8"/>
-    <mergeCell ref="C7:D7"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="K7:L7"/>
     <mergeCell ref="K9:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>